<commit_message>
Updated dependencies and Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HRMSEmployeesData.xlsx
+++ b/src/test/resources/testdata/HRMSEmployeesData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDA64B7C-0980-4F05-8BBC-787CAEF7C0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magre\IdeaProjects\HRMSB16\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5DFAB0-156C-4A22-B73C-0878FA28F7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,11 +412,11 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>